<commit_message>
Scrum Board 1 and work breakdown update
</commit_message>
<xml_diff>
--- a/Project_Management/Work breakdown structure.xlsx
+++ b/Project_Management/Work breakdown structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgsi\IdeaProjects\SE2324_63191_63324-62654_63069_62551_62482\Project_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1E75DC-9610-4448-88EA-035D81E5128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39704917-7BCE-4FC5-8B9F-5E906446C4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7104" yWindow="8964" windowWidth="23040" windowHeight="11532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Tasks:</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>First quick look at the code</t>
+  </si>
+  <si>
+    <t>Create User Stories</t>
   </si>
 </sst>
 </file>
@@ -383,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:C8"/>
+  <dimension ref="B3:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,6 +428,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>